<commit_message>
Updated 'User Stories' section in README.md. Updated 'Database collections' spreadsheet to accommodate recipe reviews.
</commit_message>
<xml_diff>
--- a/_Project Documentation/Database collections - Baking Hot.xlsx
+++ b/_Project Documentation/Database collections - Baking Hot.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="21015" windowHeight="9990"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="21015" windowHeight="9990" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Recipe Types" sheetId="2" r:id="rId1"/>
-    <sheet name="Recipes " sheetId="1" r:id="rId2"/>
-    <sheet name="Users" sheetId="3" r:id="rId3"/>
+    <sheet name="Users" sheetId="3" r:id="rId1"/>
+    <sheet name="Recipe Types" sheetId="2" r:id="rId2"/>
+    <sheet name="Recipes " sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="33">
   <si>
     <t>type</t>
   </si>
@@ -82,6 +82,39 @@
   </si>
   <si>
     <t>Collection: users</t>
+  </si>
+  <si>
+    <t>Object</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>reviews</t>
+  </si>
+  <si>
+    <t>review_text</t>
+  </si>
+  <si>
+    <t>reviewed_by</t>
+  </si>
+  <si>
+    <t>review_date</t>
+  </si>
+  <si>
+    <t>celsius</t>
+  </si>
+  <si>
+    <t>celsius_fan</t>
+  </si>
+  <si>
+    <t>fahrenheit</t>
+  </si>
+  <si>
+    <t>gas_mark</t>
   </si>
 </sst>
 </file>
@@ -431,9 +464,89 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -479,17 +592,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
@@ -497,12 +611,12 @@
     <col min="8" max="8" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1">
+    <row r="1" spans="1:3" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="2" customFormat="1">
+    <row r="2" spans="1:3" s="2" customFormat="1">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -510,7 +624,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -518,7 +632,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -526,7 +640,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -534,7 +648,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -542,7 +656,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -550,43 +664,110 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="C18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="C19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="C20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" t="s">
         <v>13</v>
       </c>
     </row>
@@ -594,66 +775,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="1"/>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>